<commit_message>
First expenses post, draft
</commit_message>
<xml_diff>
--- a/_drafts/road-trip/money.xlsx
+++ b/_drafts/road-trip/money.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claire/github/cduvallet.github.io/_drafts/road-trip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4B2419-2F83-574A-85F7-C99EAB46ABAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEC8020-F9E7-9C4E-A436-C0486F3B5E57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="800" windowWidth="27240" windowHeight="15240" xr2:uid="{8FAF9408-D19A-4243-8293-065BE15D9914}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="112">
   <si>
     <t>date</t>
   </si>
@@ -349,6 +349,18 @@
   </si>
   <si>
     <t>burrito taco lunch</t>
+  </si>
+  <si>
+    <t>ben_or_claire</t>
+  </si>
+  <si>
+    <t>car lockout</t>
+  </si>
+  <si>
+    <t>rei (parents paid)</t>
+  </si>
+  <si>
+    <t>air mattress reimbursement</t>
   </si>
 </sst>
 </file>
@@ -701,13 +713,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266AD2DD-5AE8-BD4C-8D8D-56FFD992C74B}">
-  <dimension ref="A1:F204"/>
+  <dimension ref="A1:F208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C204" sqref="C2:C204"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -722,6 +737,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -1530,6 +1548,9 @@
       <c r="D57" t="s">
         <v>15</v>
       </c>
+      <c r="E57" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -2238,6 +2259,9 @@
       <c r="D105" t="s">
         <v>15</v>
       </c>
+      <c r="E105" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
@@ -3629,6 +3653,62 @@
       </c>
       <c r="D204" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
+        <v>43582</v>
+      </c>
+      <c r="B205" t="s">
+        <v>109</v>
+      </c>
+      <c r="C205">
+        <v>65</v>
+      </c>
+      <c r="D205" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>43510</v>
+      </c>
+      <c r="B206" t="s">
+        <v>24</v>
+      </c>
+      <c r="C206">
+        <v>352.4</v>
+      </c>
+      <c r="D206" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>43512</v>
+      </c>
+      <c r="B207" t="s">
+        <v>110</v>
+      </c>
+      <c r="C207">
+        <v>297.55</v>
+      </c>
+      <c r="D207" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>43613</v>
+      </c>
+      <c r="B208" t="s">
+        <v>111</v>
+      </c>
+      <c r="C208">
+        <v>-151.58000000000001</v>
+      </c>
+      <c r="D208" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>